<commit_message>
-> Regretion DPLKKPS131-002, DPLKKPS132-002, DPLKKPS133-002, DPLKKPS134-001, DPLKKPS154-001 -> Scripting DPLKKPS146-001 until DPLKKPS148-001
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS131_RegisKelPeserta.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS131_RegisKelPeserta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D9EB75-F2FA-4DF7-A6CD-F33315D36015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C1B60B-01B4-43B1-BEE9-F1080DBF590B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPLKKPS131-002" sheetId="3" r:id="rId1"/>
@@ -135,23 +135,23 @@
 Keterangan Register : KEP.TRX.436 Pending</t>
   </si>
   <si>
+    <t>EXPLAIN</t>
+  </si>
+  <si>
+    <t>Keluarkan Peserta Dari Kolektif</t>
+  </si>
+  <si>
+    <t>NOMOR_REKENING</t>
+  </si>
+  <si>
     <t>Username : 30603;
 Password : bni1234;
 Role : Asisten Settlement;
 Keterangan Perubahan : KEP.TRX.436;
 Pilih Perusahaan : 000000029;
-No. Rekening : 790039339;
+No. Rekening : 805255179;
 Status Register : 1 : Lanjutkan ke Verifikasi;
 Keterangan Register : KEP.TRX.436 Lanjut Verifikasi</t>
-  </si>
-  <si>
-    <t>EXPLAIN</t>
-  </si>
-  <si>
-    <t>Keluarkan Peserta Dari Kolektif</t>
-  </si>
-  <si>
-    <t>NOMOR_REKENING</t>
   </si>
 </sst>
 </file>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653A54F0-D01B-49C0-BB41-F0FC7D2164BA}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +628,7 @@
         <v>24</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>25</v>
@@ -637,7 +637,7 @@
         <v>26</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="127.5" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
         <v>18</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G2" s="3">
         <v>30603</v>
@@ -687,7 +687,7 @@
         <v>28</v>
       </c>
       <c r="P2" s="2">
-        <v>790039339</v>
+        <v>805255179</v>
       </c>
       <c r="Q2" s="2">
         <v>1</v>
@@ -696,7 +696,7 @@
         <v>29</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -729,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A75AAA4-F28F-45B6-8D73-FB1F2606A1FB}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +804,7 @@
         <v>24</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>25</v>
@@ -813,7 +813,7 @@
         <v>26</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="114.75" x14ac:dyDescent="0.25">
@@ -872,7 +872,7 @@
         <v>33</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>